<commit_message>
added all data from wold bank
</commit_message>
<xml_diff>
--- a/Data-sheet-STUDENTS.xlsx
+++ b/Data-sheet-STUDENTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data-sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="175">
   <si>
     <t xml:space="preserve">Indicator #</t>
   </si>
@@ -529,6 +529,9 @@
   </si>
   <si>
     <t xml:space="preserve">ED - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WB – IFDI NET</t>
   </si>
   <si>
     <t xml:space="preserve">WHO - </t>
@@ -560,7 +563,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.00"/>
     <numFmt numFmtId="171" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -597,6 +600,13 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -688,7 +698,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -754,6 +764,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -888,15 +902,20 @@
   </sheetPr>
   <dimension ref="A1:AR71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK3" activeCellId="0" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="14.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="14.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1177,7 +1196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="121" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1308,7 +1327,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">A3+1</f>
         <v>1</v>
@@ -1689,7 +1708,7 @@
       </c>
       <c r="AB17" s="9"/>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <f aca="false">A17+1</f>
         <v>15</v>
@@ -2911,13 +2930,15 @@
   </sheetPr>
   <dimension ref="B4:C32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="10.49"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,6 +3117,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="26" customFormat="false" ht="15.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0" t="s">
         <v>152</v>
@@ -3106,7 +3135,7 @@
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
@@ -3114,7 +3143,7 @@
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>18</v>
@@ -3122,7 +3151,7 @@
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>11</v>
@@ -3130,7 +3159,7 @@
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>19</v>
@@ -3138,7 +3167,7 @@
     </row>
     <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>20</v>
@@ -3167,12 +3196,13 @@
     <hyperlink ref="C23" r:id="rId19" display="https://data.worldbank.org/indicator/IS.RRS.GOOD.MT.K6"/>
     <hyperlink ref="C24" r:id="rId20" display="https://data.worldbank.org/indicator/IS.AIR.GOOD.MT.K1"/>
     <hyperlink ref="C25" r:id="rId21" display="https://yearbook.enerdata.net/electricity/electricity-domestic-consumption-data.html"/>
-    <hyperlink ref="C27" r:id="rId22" display="https://data.worldbank.org/indicator/NE.CON.PRVT.PP.CD"/>
-    <hyperlink ref="C28" r:id="rId23" display="https://data.worldbank.org/indicator/SH.XPD.CHEX.PP.CD"/>
-    <hyperlink ref="C29" r:id="rId24" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS"/>
-    <hyperlink ref="C30" r:id="rId25" display="https://data.worldbank.org/indicator/SP.POP.SCIE.RD.P6"/>
-    <hyperlink ref="C31" r:id="rId26" display="https://data.worldbank.org/indicator/IP.TMK.RSCT"/>
-    <hyperlink ref="C32" r:id="rId27" display="https://data.worldbank.org/indicator/IP.PAT.RESD"/>
+    <hyperlink ref="C26" r:id="rId22" display="https://data.worldbank.org/indicator/BX.KLT.DINV.WD.GD.ZS"/>
+    <hyperlink ref="C27" r:id="rId23" display="https://data.worldbank.org/indicator/NE.CON.PRVT.PP.CD"/>
+    <hyperlink ref="C28" r:id="rId24" display="https://data.worldbank.org/indicator/SH.XPD.CHEX.PP.CD"/>
+    <hyperlink ref="C29" r:id="rId25" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS"/>
+    <hyperlink ref="C30" r:id="rId26" display="https://data.worldbank.org/indicator/SP.POP.SCIE.RD.P6"/>
+    <hyperlink ref="C31" r:id="rId27" display="https://data.worldbank.org/indicator/IP.TMK.RSCT"/>
+    <hyperlink ref="C32" r:id="rId28" display="https://data.worldbank.org/indicator/IP.PAT.RESD"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added test on session3 - 2
</commit_message>
<xml_diff>
--- a/Data-sheet-STUDENTS.xlsx
+++ b/Data-sheet-STUDENTS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data-sheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -563,7 +563,7 @@
     <numFmt numFmtId="170" formatCode="#,##0.00"/>
     <numFmt numFmtId="171" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -600,13 +600,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -767,7 +760,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -902,8 +895,8 @@
   </sheetPr>
   <dimension ref="A1:AR71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AH1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AK3" activeCellId="0" sqref="AK3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C70" activeCellId="0" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1083,7 +1076,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
@@ -1332,7 +1325,7 @@
         <f aca="false">A3+1</f>
         <v>1</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="8"/>
@@ -1351,7 +1344,7 @@
         <f aca="false">A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="8"/>
@@ -1370,7 +1363,7 @@
         <f aca="false">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C6" s="8"/>
@@ -1389,7 +1382,7 @@
         <f aca="false">A6+1</f>
         <v>4</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="8"/>
@@ -1408,7 +1401,7 @@
         <f aca="false">A7+1</f>
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="8"/>
@@ -1427,7 +1420,7 @@
         <f aca="false">A8+1</f>
         <v>6</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C9" s="8"/>
@@ -1484,7 +1477,7 @@
         <f aca="false">A11+1</f>
         <v>9</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C12" s="8"/>
@@ -1503,7 +1496,7 @@
         <f aca="false">A12+1</f>
         <v>10</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C13" s="8"/>
@@ -1522,7 +1515,7 @@
         <f aca="false">A13+1</f>
         <v>11</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="3" t="s">
         <v>74</v>
       </c>
       <c r="C14" s="8"/>
@@ -1669,7 +1662,7 @@
         <f aca="false">A15+1</f>
         <v>13</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C16" s="8"/>
@@ -1694,7 +1687,7 @@
         <f aca="false">A16+1</f>
         <v>14</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="3" t="s">
         <v>80</v>
       </c>
       <c r="C17" s="8"/>
@@ -1713,7 +1706,7 @@
         <f aca="false">A17+1</f>
         <v>15</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C18" s="8"/>
@@ -1732,7 +1725,7 @@
         <f aca="false">A18+1</f>
         <v>16</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="3" t="s">
         <v>82</v>
       </c>
       <c r="C19" s="8"/>
@@ -1751,7 +1744,7 @@
         <f aca="false">A19+1</f>
         <v>17</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C20" s="8"/>
@@ -1770,7 +1763,7 @@
         <f aca="false">A20+1</f>
         <v>18</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C21" s="8"/>
@@ -1789,7 +1782,7 @@
         <f aca="false">A21+1</f>
         <v>19</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C22" s="8"/>
@@ -1817,7 +1810,7 @@
         <f aca="false">A22+1</f>
         <v>20</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="3" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="8"/>
@@ -1836,7 +1829,7 @@
         <f aca="false">A23+1</f>
         <v>21</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="8"/>
@@ -1870,7 +1863,7 @@
         <f aca="false">A24+1</f>
         <v>22</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="3" t="s">
         <v>88</v>
       </c>
       <c r="C25" s="8"/>
@@ -1889,7 +1882,7 @@
         <f aca="false">A25+1</f>
         <v>23</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C26" s="8"/>
@@ -1908,7 +1901,7 @@
         <f aca="false">A26+1</f>
         <v>24</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
       <c r="C27" s="8"/>
@@ -1927,7 +1920,7 @@
         <f aca="false">A27+1</f>
         <v>25</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C28" s="8"/>
@@ -1946,7 +1939,7 @@
         <f aca="false">A28+1</f>
         <v>26</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="3" t="s">
         <v>92</v>
       </c>
       <c r="C29" s="8"/>
@@ -1965,7 +1958,7 @@
         <f aca="false">A29+1</f>
         <v>27</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C30" s="8"/>
@@ -1984,7 +1977,7 @@
         <f aca="false">A30+1</f>
         <v>28</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="3" t="s">
         <v>94</v>
       </c>
       <c r="C31" s="8"/>
@@ -2003,7 +1996,7 @@
         <f aca="false">A31+1</f>
         <v>29</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C32" s="8"/>
@@ -2022,7 +2015,7 @@
         <f aca="false">A32+1</f>
         <v>30</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="3" t="s">
         <v>96</v>
       </c>
       <c r="C33" s="8"/>
@@ -2041,7 +2034,7 @@
         <f aca="false">A33+1</f>
         <v>31</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C34" s="8"/>
@@ -2060,7 +2053,7 @@
         <f aca="false">A34+1</f>
         <v>32</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="3" t="s">
         <v>98</v>
       </c>
       <c r="C35" s="8"/>
@@ -2079,7 +2072,7 @@
         <f aca="false">A35+1</f>
         <v>33</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C36" s="8"/>
@@ -2098,7 +2091,7 @@
         <f aca="false">A36+1</f>
         <v>34</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="3" t="s">
         <v>100</v>
       </c>
       <c r="C37" s="8"/>
@@ -2117,7 +2110,7 @@
         <f aca="false">A37+1</f>
         <v>35</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C38" s="8"/>
@@ -2136,7 +2129,7 @@
         <f aca="false">A38+1</f>
         <v>36</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="3" t="s">
         <v>102</v>
       </c>
       <c r="C39" s="8"/>
@@ -2283,7 +2276,7 @@
         <f aca="false">A40+1</f>
         <v>38</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="3" t="s">
         <v>106</v>
       </c>
       <c r="C41" s="8"/>
@@ -2302,7 +2295,7 @@
         <f aca="false">A41+1</f>
         <v>39</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="3" t="s">
         <v>107</v>
       </c>
       <c r="C42" s="8"/>
@@ -2321,7 +2314,7 @@
         <f aca="false">A42+1</f>
         <v>40</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="3" t="s">
         <v>108</v>
       </c>
       <c r="C43" s="8"/>
@@ -2340,7 +2333,7 @@
         <f aca="false">A43+1</f>
         <v>41</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C44" s="8"/>
@@ -2359,7 +2352,7 @@
         <f aca="false">A44+1</f>
         <v>42</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="3" t="s">
         <v>110</v>
       </c>
       <c r="C45" s="8"/>
@@ -2378,7 +2371,7 @@
         <f aca="false">A45+1</f>
         <v>43</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C46" s="8"/>
@@ -2397,7 +2390,7 @@
         <f aca="false">A46+1</f>
         <v>44</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C47" s="8"/>
@@ -2416,7 +2409,7 @@
         <f aca="false">A47+1</f>
         <v>45</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C48" s="8"/>
@@ -2435,7 +2428,7 @@
         <f aca="false">A48+1</f>
         <v>46</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="3" t="s">
         <v>114</v>
       </c>
       <c r="C49" s="8"/>
@@ -2454,7 +2447,7 @@
         <f aca="false">A49+1</f>
         <v>47</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C50" s="8"/>
@@ -2473,7 +2466,7 @@
         <f aca="false">A50+1</f>
         <v>48</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="3" t="s">
         <v>116</v>
       </c>
       <c r="C51" s="8"/>
@@ -2492,7 +2485,7 @@
         <f aca="false">A51+1</f>
         <v>49</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C52" s="8"/>
@@ -2511,7 +2504,7 @@
         <f aca="false">A52+1</f>
         <v>50</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="3" t="s">
         <v>118</v>
       </c>
       <c r="C53" s="8"/>
@@ -2530,7 +2523,7 @@
         <f aca="false">A53+1</f>
         <v>51</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C54" s="8"/>
@@ -2549,7 +2542,7 @@
         <f aca="false">A54+1</f>
         <v>52</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="3" t="s">
         <v>120</v>
       </c>
       <c r="C55" s="8"/>
@@ -2568,7 +2561,7 @@
         <f aca="false">A55+1</f>
         <v>53</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C56" s="8"/>
@@ -2587,7 +2580,7 @@
         <f aca="false">A56+1</f>
         <v>54</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="3" t="s">
         <v>122</v>
       </c>
       <c r="C57" s="8"/>
@@ -2606,7 +2599,7 @@
         <f aca="false">A57+1</f>
         <v>55</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C58" s="8"/>
@@ -2625,7 +2618,7 @@
         <f aca="false">A58+1</f>
         <v>56</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="3" t="s">
         <v>124</v>
       </c>
       <c r="C59" s="8"/>
@@ -2644,7 +2637,7 @@
         <f aca="false">A59+1</f>
         <v>57</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C60" s="8"/>
@@ -2663,7 +2656,7 @@
         <f aca="false">A60+1</f>
         <v>58</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="3" t="s">
         <v>126</v>
       </c>
       <c r="C61" s="8"/>
@@ -2682,7 +2675,7 @@
         <f aca="false">A61+1</f>
         <v>59</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C62" s="8"/>
@@ -2704,7 +2697,7 @@
         <f aca="false">A62+1</f>
         <v>60</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="3" t="s">
         <v>128</v>
       </c>
       <c r="C63" s="8"/>
@@ -2723,7 +2716,7 @@
         <f aca="false">A63+1</f>
         <v>61</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C64" s="8"/>
@@ -2742,7 +2735,7 @@
         <f aca="false">A64+1</f>
         <v>62</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="3" t="s">
         <v>130</v>
       </c>
       <c r="C65" s="8"/>
@@ -2761,7 +2754,7 @@
         <f aca="false">A65+1</f>
         <v>63</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C66" s="8"/>
@@ -2783,7 +2776,7 @@
         <f aca="false">A66+1</f>
         <v>64</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="3" t="s">
         <v>132</v>
       </c>
       <c r="C67" s="8"/>
@@ -2802,7 +2795,7 @@
         <f aca="false">A67+1</f>
         <v>65</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C68" s="8"/>
@@ -2821,7 +2814,7 @@
         <f aca="false">A68+1</f>
         <v>66</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="3" t="s">
         <v>134</v>
       </c>
       <c r="C69" s="8"/>
@@ -2875,40 +2868,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://www.heritage.org/index/"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://www.heritage.org/index/"/>
-    <hyperlink ref="F2" r:id="rId3" display="https://www.bti-project.org/en/home/"/>
-    <hyperlink ref="G2" r:id="rId4" display="https://www.bti-project.org/en/home/"/>
-    <hyperlink ref="H2" r:id="rId5" display="https://data.worldbank.org/indicator/GC.TAX.IMPT.ZS"/>
-    <hyperlink ref="I2" r:id="rId6" display="https://data.worldbank.org/indicator/FB.AST.NPER.ZS"/>
-    <hyperlink ref="J2" r:id="rId7" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
-    <hyperlink ref="K2" r:id="rId8" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
-    <hyperlink ref="L2" r:id="rId9" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
-    <hyperlink ref="M2" r:id="rId10" display="https://data.worldbank.org/indicator/IS.RRS.GOOD.MT.K6"/>
-    <hyperlink ref="N2" r:id="rId11" display="https://data.worldbank.org/indicator/IS.RRS.GOOD.MT.K6"/>
-    <hyperlink ref="O2" r:id="rId12" display="https://data.worldbank.org/indicator/NE.CON.PRVT.PP.CD"/>
-    <hyperlink ref="P2" r:id="rId13" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS?locations=MY-KH"/>
-    <hyperlink ref="Q2" r:id="rId14" display="https://data.worldbank.org/indicator/SP.POP.SCIE.RD.P6"/>
-    <hyperlink ref="R2" r:id="rId15" display="https://www.transparency.org/research/cpi/overview"/>
-    <hyperlink ref="S2" r:id="rId16" display="https://www.transparency.org/research/cpi/overview"/>
-    <hyperlink ref="T2" r:id="rId17" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="U2" r:id="rId18" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="V2" r:id="rId19" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="W2" r:id="rId20" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="X2" r:id="rId21" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="Y2" r:id="rId22" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="Z2" r:id="rId23" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="AB2" r:id="rId24" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="AD2" r:id="rId25" display="https://wits.worldbank.org/country-indicator.aspx?lang=en"/>
-    <hyperlink ref="AG2" r:id="rId26" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="AH2" r:id="rId27" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="AI2" r:id="rId28" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
-    <hyperlink ref="AM2" r:id="rId29" display="https://data.worldbank.org/indicator/BX.KLT.DINV.WD.GD.ZS"/>
-    <hyperlink ref="AN2" r:id="rId30" display="https://yearbook.enerdata.net/electricity/electricity-domestic-consumption-data.html"/>
-    <hyperlink ref="AO2" r:id="rId31" display="https://data.worldbank.org/indicator/SH.XPD.CHEX.PP.CD"/>
-    <hyperlink ref="AP2" r:id="rId32" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS"/>
-    <hyperlink ref="AQ2" r:id="rId33" display="https://data.worldbank.org/indicator/IP.TMK.RSCT"/>
-    <hyperlink ref="AR2" r:id="rId34" display="https://data.worldbank.org/indicator/IP.PAT.RESD"/>
+    <hyperlink ref="E2" r:id="rId1" display="https://www.heritage.org/index/"/>
+    <hyperlink ref="F2" r:id="rId2" display="https://www.bti-project.org/en/home/"/>
+    <hyperlink ref="G2" r:id="rId3" display="https://www.bti-project.org/en/home/"/>
+    <hyperlink ref="H2" r:id="rId4" display="https://data.worldbank.org/indicator/GC.TAX.IMPT.ZS"/>
+    <hyperlink ref="I2" r:id="rId5" display="https://data.worldbank.org/indicator/FB.AST.NPER.ZS"/>
+    <hyperlink ref="J2" r:id="rId6" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
+    <hyperlink ref="K2" r:id="rId7" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
+    <hyperlink ref="L2" r:id="rId8" display="https://globalratings.net/ratings-info/rating-scales-definitions"/>
+    <hyperlink ref="M2" r:id="rId9" display="https://data.worldbank.org/indicator/IS.RRS.GOOD.MT.K6"/>
+    <hyperlink ref="N2" r:id="rId10" display="https://data.worldbank.org/indicator/IS.RRS.GOOD.MT.K6"/>
+    <hyperlink ref="O2" r:id="rId11" display="https://data.worldbank.org/indicator/NE.CON.PRVT.PP.CD"/>
+    <hyperlink ref="P2" r:id="rId12" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS?locations=MY-KH"/>
+    <hyperlink ref="Q2" r:id="rId13" display="https://data.worldbank.org/indicator/SP.POP.SCIE.RD.P6"/>
+    <hyperlink ref="R2" r:id="rId14" display="https://www.transparency.org/research/cpi/overview"/>
+    <hyperlink ref="S2" r:id="rId15" display="https://www.transparency.org/research/cpi/overview"/>
+    <hyperlink ref="T2" r:id="rId16" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="U2" r:id="rId17" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="V2" r:id="rId18" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="W2" r:id="rId19" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="X2" r:id="rId20" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="Y2" r:id="rId21" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="Z2" r:id="rId22" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="AB2" r:id="rId23" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="AD2" r:id="rId24" display="https://wits.worldbank.org/country-indicator.aspx?lang=en"/>
+    <hyperlink ref="AG2" r:id="rId25" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="AH2" r:id="rId26" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="AI2" r:id="rId27" display="https://eng.yidaiyilu.gov.cn/jcsuce.htm?0"/>
+    <hyperlink ref="AM2" r:id="rId28" display="https://data.worldbank.org/indicator/BX.KLT.DINV.WD.GD.ZS"/>
+    <hyperlink ref="AN2" r:id="rId29" display="https://yearbook.enerdata.net/electricity/electricity-domestic-consumption-data.html"/>
+    <hyperlink ref="AO2" r:id="rId30" display="https://data.worldbank.org/indicator/SH.XPD.CHEX.PP.CD"/>
+    <hyperlink ref="AP2" r:id="rId31" display="https://data.worldbank.org/indicator/GB.XPD.RSDV.GD.ZS"/>
+    <hyperlink ref="AQ2" r:id="rId32" display="https://data.worldbank.org/indicator/IP.TMK.RSCT"/>
+    <hyperlink ref="AR2" r:id="rId33" display="https://data.worldbank.org/indicator/IP.PAT.RESD"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2918,7 +2910,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId35"/>
+    <tablePart r:id="rId34"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2930,7 +2922,7 @@
   </sheetPr>
   <dimension ref="B4:C32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>